<commit_message>
Risk Assessment completed and exported
</commit_message>
<xml_diff>
--- a/Documentation/risk-assessment.xlsx
+++ b/Documentation/risk-assessment.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/384d642e32fda18f/Software/QA/Projects/2-coreProject/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmmyB.000\Desktop\OneDrive\Software\QA\Projects\2-coreProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="11_F25DC773A252ABDACC1048AB01DD766A5ADE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B217B906-7F0E-4E92-9A0D-F038BC53D1E7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68697E58-2210-4896-94AF-D2FAB907AAC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
   <si>
     <t>VERY LOW (1)</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>DID IT HAPPEN?</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -513,14 +516,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -577,6 +574,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -892,18 +895,18 @@
     <row r="3" spans="2:13" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="14"/>
       <c r="C3" s="15"/>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
       <c r="K3" s="15"/>
       <c r="L3" s="15"/>
-      <c r="M3" s="17"/>
+      <c r="M3" s="16"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="14"/>
@@ -917,7 +920,7 @@
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>
-      <c r="M4" s="17"/>
+      <c r="M4" s="16"/>
     </row>
     <row r="5" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="14"/>
@@ -941,7 +944,7 @@
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
-      <c r="M5" s="17"/>
+      <c r="M5" s="16"/>
     </row>
     <row r="6" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="14"/>
@@ -964,14 +967,14 @@
         <v>5</v>
       </c>
       <c r="I6" s="15"/>
-      <c r="J6" s="18" t="s">
+      <c r="J6" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="K6" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="19"/>
-      <c r="M6" s="17"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="16"/>
     </row>
     <row r="7" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="14"/>
@@ -994,14 +997,14 @@
         <v>10</v>
       </c>
       <c r="I7" s="15"/>
-      <c r="J7" s="20" t="s">
+      <c r="J7" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="K7" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="19"/>
-      <c r="M7" s="17"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="16"/>
     </row>
     <row r="8" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="14"/>
@@ -1024,14 +1027,14 @@
         <v>15</v>
       </c>
       <c r="I8" s="15"/>
-      <c r="J8" s="21" t="s">
+      <c r="J8" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="19" t="s">
+      <c r="K8" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="L8" s="19"/>
-      <c r="M8" s="17"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="16"/>
     </row>
     <row r="9" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="14"/>
@@ -1054,14 +1057,14 @@
         <v>20</v>
       </c>
       <c r="I9" s="15"/>
-      <c r="J9" s="22" t="s">
+      <c r="J9" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="K9" s="19" t="s">
+      <c r="K9" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="L9" s="19"/>
-      <c r="M9" s="17"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="16"/>
     </row>
     <row r="10" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="14"/>
@@ -1084,14 +1087,14 @@
         <v>25</v>
       </c>
       <c r="I10" s="15"/>
-      <c r="J10" s="23" t="s">
+      <c r="J10" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="K10" s="19" t="s">
+      <c r="K10" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="L10" s="19"/>
-      <c r="M10" s="17"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="16"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="14"/>
@@ -1105,30 +1108,30 @@
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
       <c r="L11" s="15"/>
-      <c r="M11" s="17"/>
+      <c r="M11" s="16"/>
     </row>
     <row r="12" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="24"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="26"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="K10:L10"/>
     <mergeCell ref="D3:J3"/>
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="K7:L7"/>
     <mergeCell ref="K8:L8"/>
     <mergeCell ref="K9:L9"/>
-    <mergeCell ref="K10:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1145,7 +1148,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.140625" style="28"/>
+    <col min="2" max="2" width="9.140625" style="26"/>
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
@@ -1157,8 +1160,8 @@
     <col min="12" max="12" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:13" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:13" s="26" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:13" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="11"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
@@ -1175,20 +1178,20 @@
     <row r="3" spans="2:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="14"/>
       <c r="C3" s="15"/>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
       <c r="K3" s="15"/>
       <c r="L3" s="15"/>
-      <c r="M3" s="17"/>
-    </row>
-    <row r="4" spans="2:13" s="28" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M3" s="16"/>
+    </row>
+    <row r="4" spans="2:13" s="26" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="14"/>
       <c r="C4" s="15"/>
       <c r="D4" s="15"/>
@@ -1200,191 +1203,191 @@
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>
-      <c r="M4" s="17"/>
+      <c r="M4" s="16"/>
     </row>
     <row r="5" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="14"/>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="31" t="s">
+      <c r="F5" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="31" t="s">
+      <c r="G5" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="31" t="s">
+      <c r="H5" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="31" t="s">
+      <c r="I5" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="31" t="s">
+      <c r="J5" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="K5" s="31" t="s">
+      <c r="K5" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="L5" s="31" t="s">
+      <c r="L5" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="M5" s="17"/>
+      <c r="M5" s="16"/>
     </row>
     <row r="6" spans="2:13" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="14"/>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="32">
         <v>2</v>
       </c>
-      <c r="F6" s="34">
+      <c r="F6" s="32">
         <v>5</v>
       </c>
-      <c r="G6" s="36">
+      <c r="G6" s="34">
         <v>10</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="H6" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="30" t="s">
+      <c r="I6" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="J6" s="34">
+      <c r="J6" s="32">
         <v>1</v>
       </c>
-      <c r="K6" s="34">
-        <v>4</v>
-      </c>
-      <c r="L6" s="32">
-        <v>4</v>
-      </c>
-      <c r="M6" s="17"/>
+      <c r="K6" s="32">
+        <v>4</v>
+      </c>
+      <c r="L6" s="30">
+        <v>4</v>
+      </c>
+      <c r="M6" s="16"/>
     </row>
     <row r="7" spans="2:13" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="14"/>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="35">
+      <c r="E7" s="33">
         <v>3</v>
       </c>
-      <c r="F7" s="35">
-        <v>4</v>
-      </c>
-      <c r="G7" s="38">
+      <c r="F7" s="33">
+        <v>4</v>
+      </c>
+      <c r="G7" s="36">
         <v>12</v>
       </c>
-      <c r="H7" s="29" t="s">
+      <c r="H7" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="29" t="s">
+      <c r="I7" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="35">
+      <c r="J7" s="33">
         <v>2</v>
       </c>
-      <c r="K7" s="35">
+      <c r="K7" s="33">
         <v>2</v>
       </c>
-      <c r="L7" s="33">
-        <v>4</v>
-      </c>
-      <c r="M7" s="17"/>
+      <c r="L7" s="31">
+        <v>4</v>
+      </c>
+      <c r="M7" s="16"/>
     </row>
     <row r="8" spans="2:13" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="14"/>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="35">
-        <v>4</v>
-      </c>
-      <c r="F8" s="35">
+      <c r="E8" s="33">
+        <v>4</v>
+      </c>
+      <c r="F8" s="33">
         <v>5</v>
       </c>
-      <c r="G8" s="39">
+      <c r="G8" s="37">
         <v>20</v>
       </c>
-      <c r="H8" s="29" t="s">
+      <c r="H8" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="29" t="s">
+      <c r="I8" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="35">
+      <c r="J8" s="33">
         <v>3</v>
       </c>
-      <c r="K8" s="35">
-        <v>4</v>
-      </c>
-      <c r="L8" s="38">
+      <c r="K8" s="33">
+        <v>4</v>
+      </c>
+      <c r="L8" s="36">
         <v>12</v>
       </c>
-      <c r="M8" s="17"/>
+      <c r="M8" s="16"/>
     </row>
     <row r="9" spans="2:13" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="14"/>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="35">
+      <c r="E9" s="33">
         <v>2</v>
       </c>
-      <c r="F9" s="35">
-        <v>4</v>
-      </c>
-      <c r="G9" s="37">
+      <c r="F9" s="33">
+        <v>4</v>
+      </c>
+      <c r="G9" s="35">
         <v>8</v>
       </c>
-      <c r="H9" s="29" t="s">
+      <c r="H9" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="I9" s="29" t="s">
+      <c r="I9" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="35">
+      <c r="J9" s="33">
         <v>1</v>
       </c>
-      <c r="K9" s="35">
-        <v>4</v>
-      </c>
-      <c r="L9" s="33">
-        <v>4</v>
-      </c>
-      <c r="M9" s="17"/>
+      <c r="K9" s="33">
+        <v>4</v>
+      </c>
+      <c r="L9" s="31">
+        <v>4</v>
+      </c>
+      <c r="M9" s="16"/>
     </row>
     <row r="10" spans="2:13" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="24"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="26"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1399,22 +1402,22 @@
   <dimension ref="B1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="28"/>
-    <col min="3" max="3" width="12.5703125" style="28" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="28" customWidth="1"/>
-    <col min="5" max="5" width="13" style="28" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="28" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="28" customWidth="1"/>
-    <col min="8" max="9" width="14.140625" style="28" customWidth="1"/>
-    <col min="10" max="10" width="13" style="28" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" style="28" customWidth="1"/>
-    <col min="12" max="14" width="10.7109375" style="28" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="28"/>
+    <col min="1" max="2" width="9.140625" style="26"/>
+    <col min="3" max="3" width="12.5703125" style="26" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="26" customWidth="1"/>
+    <col min="5" max="5" width="13" style="26" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="26" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="26" customWidth="1"/>
+    <col min="8" max="9" width="14.140625" style="26" customWidth="1"/>
+    <col min="10" max="10" width="13" style="26" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" style="26" customWidth="1"/>
+    <col min="12" max="14" width="10.7109375" style="26" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1437,19 +1440,19 @@
     <row r="3" spans="2:15" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="14"/>
       <c r="C3" s="15"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="16" t="s">
+      <c r="E3" s="25"/>
+      <c r="F3" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
       <c r="K3" s="15"/>
       <c r="L3" s="15"/>
       <c r="M3" s="15"/>
       <c r="N3" s="15"/>
-      <c r="O3" s="17"/>
+      <c r="O3" s="16"/>
     </row>
     <row r="4" spans="2:15" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="14"/>
@@ -1465,219 +1468,227 @@
       <c r="L4" s="15"/>
       <c r="M4" s="15"/>
       <c r="N4" s="15"/>
-      <c r="O4" s="17"/>
+      <c r="O4" s="16"/>
     </row>
     <row r="5" spans="2:15" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="14"/>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="31" t="s">
+      <c r="F5" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="31" t="s">
+      <c r="G5" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="31" t="s">
+      <c r="H5" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="31" t="s">
+      <c r="I5" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="31" t="s">
+      <c r="J5" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="K5" s="31" t="s">
+      <c r="K5" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="L5" s="31" t="s">
+      <c r="L5" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="M5" s="40" t="s">
+      <c r="M5" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="N5" s="40" t="s">
+      <c r="N5" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="17"/>
+      <c r="O5" s="16"/>
     </row>
     <row r="6" spans="2:15" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="14"/>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="32">
         <v>2</v>
       </c>
-      <c r="F6" s="34">
+      <c r="F6" s="32">
         <v>5</v>
       </c>
-      <c r="G6" s="36">
+      <c r="G6" s="34">
         <v>10</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="H6" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="30" t="s">
+      <c r="I6" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="J6" s="34">
+      <c r="J6" s="32">
         <v>1</v>
       </c>
-      <c r="K6" s="34">
-        <v>4</v>
-      </c>
-      <c r="L6" s="32">
-        <v>4</v>
-      </c>
-      <c r="M6" s="35"/>
-      <c r="N6" s="35" t="str">
+      <c r="K6" s="32">
+        <v>4</v>
+      </c>
+      <c r="L6" s="30">
+        <v>4</v>
+      </c>
+      <c r="M6" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="N6" s="33" t="str">
         <f>IF(M6="no", "n/a", " … ")</f>
-        <v xml:space="preserve"> … </v>
-      </c>
-      <c r="O6" s="17"/>
+        <v>n/a</v>
+      </c>
+      <c r="O6" s="16"/>
     </row>
     <row r="7" spans="2:15" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="14"/>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="35">
+      <c r="E7" s="33">
         <v>3</v>
       </c>
-      <c r="F7" s="35">
-        <v>4</v>
-      </c>
-      <c r="G7" s="38">
+      <c r="F7" s="33">
+        <v>4</v>
+      </c>
+      <c r="G7" s="36">
         <v>12</v>
       </c>
-      <c r="H7" s="29" t="s">
+      <c r="H7" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="29" t="s">
+      <c r="I7" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="35">
+      <c r="J7" s="33">
         <v>2</v>
       </c>
-      <c r="K7" s="35">
+      <c r="K7" s="33">
         <v>2</v>
       </c>
-      <c r="L7" s="33">
-        <v>4</v>
-      </c>
-      <c r="M7" s="35"/>
-      <c r="N7" s="35" t="str">
+      <c r="L7" s="31">
+        <v>4</v>
+      </c>
+      <c r="M7" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="N7" s="33" t="str">
         <f t="shared" ref="N7:N9" si="0">IF(M7="no", "n/a", " … ")</f>
-        <v xml:space="preserve"> … </v>
-      </c>
-      <c r="O7" s="17"/>
+        <v>n/a</v>
+      </c>
+      <c r="O7" s="16"/>
     </row>
     <row r="8" spans="2:15" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="14"/>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="35">
-        <v>4</v>
-      </c>
-      <c r="F8" s="35">
+      <c r="E8" s="33">
+        <v>4</v>
+      </c>
+      <c r="F8" s="33">
         <v>5</v>
       </c>
-      <c r="G8" s="39">
+      <c r="G8" s="37">
         <v>20</v>
       </c>
-      <c r="H8" s="29" t="s">
+      <c r="H8" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="29" t="s">
+      <c r="I8" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="35">
+      <c r="J8" s="33">
         <v>3</v>
       </c>
-      <c r="K8" s="35">
-        <v>4</v>
-      </c>
-      <c r="L8" s="38">
+      <c r="K8" s="33">
+        <v>4</v>
+      </c>
+      <c r="L8" s="36">
         <v>12</v>
       </c>
-      <c r="M8" s="35"/>
-      <c r="N8" s="35" t="str">
+      <c r="M8" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="N8" s="33" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> … </v>
-      </c>
-      <c r="O8" s="17"/>
+        <v>n/a</v>
+      </c>
+      <c r="O8" s="16"/>
     </row>
     <row r="9" spans="2:15" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="14"/>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="35">
+      <c r="E9" s="33">
         <v>2</v>
       </c>
-      <c r="F9" s="35">
-        <v>4</v>
-      </c>
-      <c r="G9" s="37">
+      <c r="F9" s="33">
+        <v>4</v>
+      </c>
+      <c r="G9" s="35">
         <v>8</v>
       </c>
-      <c r="H9" s="29" t="s">
+      <c r="H9" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="I9" s="29" t="s">
+      <c r="I9" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="35">
+      <c r="J9" s="33">
         <v>1</v>
       </c>
-      <c r="K9" s="35">
-        <v>4</v>
-      </c>
-      <c r="L9" s="33">
-        <v>4</v>
-      </c>
-      <c r="M9" s="35"/>
-      <c r="N9" s="35" t="str">
+      <c r="K9" s="33">
+        <v>4</v>
+      </c>
+      <c r="L9" s="31">
+        <v>4</v>
+      </c>
+      <c r="M9" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="N9" s="33" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> … </v>
-      </c>
-      <c r="O9" s="17"/>
+        <v>n/a</v>
+      </c>
+      <c r="O9" s="16"/>
     </row>
     <row r="10" spans="2:15" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="24"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="26"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>